<commit_message>
add bst and binary heap
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK221\SoftwareTest\AutoTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hk221\Software Testing\AutoTest-main\AutoTest-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3810FFE2-CD27-4AD1-B16B-BA0FC38797A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B7A276-FF35-40AA-B91F-613840BA0B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="22" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sort" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,29 @@
     <sheet name="LinkedList_Search_Result" sheetId="8" r:id="rId8"/>
     <sheet name="LinkedList_Remove" sheetId="9" r:id="rId9"/>
     <sheet name="LinkedList_Remove_Result" sheetId="10" r:id="rId10"/>
+    <sheet name="BST_Create" sheetId="11" r:id="rId11"/>
+    <sheet name="BST_Create_Result" sheetId="12" r:id="rId12"/>
+    <sheet name="BST_Insert" sheetId="13" r:id="rId13"/>
+    <sheet name="BST_Insert_Result" sheetId="14" r:id="rId14"/>
+    <sheet name="BST_Search" sheetId="15" r:id="rId15"/>
+    <sheet name="BST_Search_Result" sheetId="16" r:id="rId16"/>
+    <sheet name="BST_Remove" sheetId="17" r:id="rId17"/>
+    <sheet name="BST_Remove_Result" sheetId="18" r:id="rId18"/>
+    <sheet name="BinaryHeap_Create" sheetId="19" r:id="rId19"/>
+    <sheet name="BinaryHeap_Create_Result" sheetId="20" r:id="rId20"/>
+    <sheet name="BinaryHeap_Insert" sheetId="21" r:id="rId21"/>
+    <sheet name="BinaryHeap_Insert_Result" sheetId="22" r:id="rId22"/>
+    <sheet name="BinaryHeap_Update" sheetId="23" r:id="rId23"/>
+    <sheet name="BinaryHeap_Update_Result" sheetId="24" r:id="rId24"/>
+    <sheet name="BinaryHeap_Delete" sheetId="25" r:id="rId25"/>
+    <sheet name="BinaryHeap_Delete_Result" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="88">
   <si>
     <t>Testcase</t>
   </si>
@@ -181,17 +197,134 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>BST_Create</t>
+  </si>
+  <si>
+    <t>BST_Insert</t>
+  </si>
+  <si>
+    <t>Sorry, only values between 1 and 100 can be inserted.</t>
+  </si>
+  <si>
+    <t>2,3,6,8,99,88,55</t>
+  </si>
+  <si>
+    <t>Please fill in a number or comma-separated array of numbers!</t>
+  </si>
+  <si>
+    <t>2, 2</t>
+  </si>
+  <si>
+    <t>No duplicate vertex allowed!</t>
+  </si>
+  <si>
+    <t>BST_Search</t>
+  </si>
+  <si>
+    <t>Found value 78.0</t>
+  </si>
+  <si>
+    <t>Found value 22.0.</t>
+  </si>
+  <si>
+    <t>Found value 81.0</t>
+  </si>
+  <si>
+    <t>Value -1.0 is not in the BST.</t>
+  </si>
+  <si>
+    <t>Value is not in the BST.</t>
+  </si>
+  <si>
+    <t>Found value 78.0.</t>
+  </si>
+  <si>
+    <t>Value 22.0 is not in the BST.</t>
+  </si>
+  <si>
+    <t>Value 81.0 is not in the BST.</t>
+  </si>
+  <si>
+    <t>BST_Remove</t>
+  </si>
+  <si>
+    <t>2,7,26,25,19,17,1,90,3,36</t>
+  </si>
+  <si>
+    <t>The Binary Max Heap has been successfully created from array A: 2,7,26,25,19,17,1,90,3,36.</t>
+  </si>
+  <si>
+    <t>The Binary Max Heap has been successfully created from array A: 1.</t>
+  </si>
+  <si>
+    <t>-1,-2,-3</t>
+  </si>
+  <si>
+    <t>The Binary Max Heap has been successfully created from array A: -1,-2,-3.</t>
+  </si>
+  <si>
+    <t>The Binary Max Heap has been successfully created from array A: .</t>
+  </si>
+  <si>
+    <t>The Binary Max Heap has been successfully created from array A: ,.</t>
+  </si>
+  <si>
+    <t>1,2,2</t>
+  </si>
+  <si>
+    <t>The Binary Max Heap has been successfully created from array A: 1,2,2.</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16</t>
+  </si>
+  <si>
+    <t>The Binary Max Heap has been successfully created from array A: 1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16.</t>
+  </si>
+  <si>
+    <t>BinaryHeap_Insert</t>
+  </si>
+  <si>
+    <t>-222</t>
+  </si>
+  <si>
+    <t>v must be ∈ [-99..99]</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>BinaryHeap_Update</t>
+  </si>
+  <si>
+    <t>newv must be ∈ [-99..99]</t>
+  </si>
+  <si>
+    <t>BinaryHeap_Delete</t>
+  </si>
+  <si>
+    <t>i must be ∈ [1..7]</t>
+  </si>
+  <si>
+    <t>i must be ∈ [1..10]</t>
+  </si>
+  <si>
+    <t>i must be ∈ [1..12]</t>
+  </si>
+  <si>
+    <t>i must be ∈ [1..6]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -225,6 +358,41 @@
       <sz val="11"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -234,7 +402,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -332,11 +500,116 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -365,6 +638,27 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -672,13 +966,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="38.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +992,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -712,7 +1006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -726,7 +1020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -740,7 +1034,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -754,7 +1048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -768,7 +1062,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -782,7 +1076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -796,7 +1090,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -810,7 +1104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -821,7 +1115,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -845,19 +1139,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="A1:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="34.296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -877,7 +1171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -897,7 +1191,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -917,7 +1211,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -937,7 +1231,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -954,7 +1248,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -971,7 +1265,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -990,6 +1284,1031 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="38.21875" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="41.6640625" customWidth="1"/>
+    <col min="5" max="5" width="43.33203125" customWidth="1"/>
+    <col min="6" max="6" width="38.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="54.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="5" width="52.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4">
+        <v>-1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45" customWidth="1"/>
+    <col min="4" max="4" width="86.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -999,9 +2318,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +2340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1038,7 +2357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1055,7 +2374,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1072,7 +2391,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1092,7 +2411,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1112,7 +2431,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1129,7 +2448,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1149,7 +2468,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1169,7 +2488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1186,7 +2505,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1201,6 +2520,897 @@
       </c>
       <c r="F11" t="s">
         <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="4" max="4" width="52.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="35.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="5" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2">
+        <v>-222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5">
+        <v>999</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="39.21875" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2">
+        <v>-222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5">
+        <v>999</v>
+      </c>
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="38.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="33.77734375" customWidth="1"/>
+    <col min="5" max="5" width="30.88671875" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2">
+        <v>-222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5">
+        <v>999</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1213,20 +3423,20 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="F8" sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.09765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +3456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1260,7 +3470,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1274,7 +3484,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1288,7 +3498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1299,7 +3509,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1313,7 +3523,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1327,7 +3537,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1355,15 +3565,15 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="42.09765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +3593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1400,7 +3610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1417,7 +3627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1434,7 +3644,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1451,7 +3661,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1468,7 +3678,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1485,7 +3695,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1515,17 +3725,17 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1545,7 +3755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1559,7 +3769,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1573,7 +3783,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1587,7 +3797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1601,7 +3811,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1613,7 +3823,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
     </row>
   </sheetData>
@@ -1630,15 +3840,15 @@
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="34.296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1658,7 +3868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1678,7 +3888,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1695,7 +3905,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1712,7 +3922,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1732,7 +3942,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1759,20 +3969,20 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="G6" sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.8984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +4002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1806,7 +4016,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1820,7 +4030,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1834,7 +4044,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1848,7 +4058,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1860,15 +4070,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <ignoredErrors>
-    <ignoredError sqref="C2:C5" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1877,18 +4084,18 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="45.59765625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="45.5546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1908,7 +4115,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1928,7 +4135,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1948,7 +4155,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1968,7 +4175,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1988,7 +4195,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2015,20 +4222,20 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection sqref="A1:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2048,7 +4255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2062,7 +4269,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2076,7 +4283,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2090,7 +4297,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2104,7 +4311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2118,7 +4325,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2130,14 +4337,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <ignoredErrors>
-    <ignoredError sqref="C2:C6" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>